<commit_message>
Topics e topic_bert added
</commit_message>
<xml_diff>
--- a/Noise_remover/tweets_processados_espanhol.xlsx
+++ b/Noise_remover/tweets_processados_espanhol.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,21 +462,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.92534571387082e+18</v>
+        <v>1.933449667456422e+18</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alguien más con neumonía? Digo para sentarnos a comer amoxilina juntos</t>
+          <t>@LeticiaFrost0 @_pao_com_banana Fui lembramdo por lele da silva yayyy https://t.co/ReFEDaDEEp</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>May 22, 2025 at 12:19 AM</t>
+          <t>June 13, 2025 at 09:01 AM</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>alguien más con neumonía digo para sentarnos a comer amoxilina juntos</t>
+          <t xml:space="preserve"> pao com banana fui lembramdo por lele da silva yayyy </t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -487,21 +487,21 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.924588836404757e+18</v>
+        <v>1.933261971622613e+18</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>@roxanacastel Para el otitis me dio amoxilina está bien eso? Ya ni en los médicos confío</t>
+          <t>@p2rcys fun fact no inverno tem aumento de casos de infeccao urinaria</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>May 19, 2025 at 10:11 PM</t>
+          <t>June 12, 2025 at 08:35 PM</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> para el otitis me dio amoxilina está bien eso ya ni en los médicos confío</t>
+          <t xml:space="preserve"> fun fact no inverno tem aumento de casos de infeccao urinaria</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -512,21 +512,21 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.924256533908525e+18</v>
+        <v>1.932477783604712e+18</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>@petrogustavo @AlvaroUribeVel @JuanManSantos @IvanDuque @FuerzasMilCol @PoliciaColombia @realDonaldTrump @VP @ONU_es señores tomo complejo b tiamina amoxilina acetaminofen para deter ese aparato lee mentes que quiere destruir a los militares policias niños de colombia ayudenme. https://t.co/cvIFAhIu1q</t>
+          <t>@ybernxd infeccao urinaria</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>May 19, 2025 at 12:11 AM</t>
+          <t>June 10, 2025 at 04:39 PM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> señores tomo complejo b tiamina amoxilina acetaminofen para deter ese aparato lee mentes que quiere destruir a los militares policias niños de colombia ayudenme </t>
+          <t xml:space="preserve"> infeccao urinaria</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -537,26 +537,21 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.923135522882392e+18</v>
+        <v>1.931740333252944e+18</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Hoy vino un veneco que ya lo tengo medio cruzado
--Que andabas buscando?
--Una "amoxilina"
--Eh... de cuanto te dio el medico?
--No es de venta libre eso?
-Una "amoxilina"...un cachetazo en la jeta te voy dar</t>
+          <t>@psyllobor4 lembrando q sodio da infeccao urinaria</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>May 15, 2025 at 09:56 PM</t>
+          <t>June 8, 2025 at 03:49 PM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>hoy vino un veneco que ya lo tengo medio cruzado que andabas buscando una "amoxilina" eh de cuanto te dio el medico no es de venta libre eso una "amoxilina" un cachetazo en la jeta te voy dar</t>
+          <t xml:space="preserve"> lembrando q sodio da infeccao urinaria</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -567,21 +562,21 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.922027126233981e+18</v>
+        <v>1.931476868613477e+18</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Preciso de amoxilina</t>
+          <t>@tudojaywon a infeccao urinaria babado</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>May 12, 2025 at 08:32 PM</t>
+          <t>June 7, 2025 at 10:22 PM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>preciso de amoxilina</t>
+          <t xml:space="preserve"> a infeccao urinaria babado</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -592,21 +587,21 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1.920588369064588e+18</v>
+        <v>1.903095762231182e+18</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Hoje a base de amoxilina e decadron</t>
+          <t>infeccao urinaria eh para poucos https://t.co/2rRhtIWgNv</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>May 8, 2025 at 09:15 PM</t>
+          <t>March 21, 2025 at 02:46 PM</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>hoje a base de amoxilina e decadro</t>
+          <t xml:space="preserve">feccao urinaria eh para poucos </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -617,22 +612,21 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.917330811994391e+18</v>
+        <v>1.884593735926797e+18</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ketarolaco y amoxilina a jugar.
-Que no mame, Carioca. 🤣</t>
+          <t>Acho q to c infeccao urinaria</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>April 29, 2025 at 09:31 PM</t>
+          <t>January 29, 2025 at 01:25 PM</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ketarolaco y amoxilina a jugar que no mame carioca 🤣</t>
+          <t>acho q to c infeccao urinaria</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -643,21 +637,21 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.916108627305186e+18</v>
+        <v>1.8843596989938e+18</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Tome la amoxilina y parece que me di un saque de lo estúpida y el sueño que tengo</t>
+          <t>acho que to infeccao urinaria</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>April 26, 2025 at 12:34 PM</t>
+          <t>January 28, 2025 at 09:55 PM</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>tome la amoxilina y parece que me di un saque de lo estúpida y el sueño que tengo</t>
+          <t>acho que to infeccao urinaria</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -668,104 +662,24 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.916096954439762e+18</v>
+        <v>1.883974742761431e+18</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>@grok @DoctorSITHo Ya está bien con el antibiótico! La amoxilina 10 días cada 8h y como nuevo. 
-Vete a tomar por el lado oscuro @grok</t>
+          <t>@conexaocec @venecasagrande DUROS</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>April 26, 2025 at 11:48 AM</t>
+          <t>January 27, 2025 at 08:25 PM</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ya está bien con el antibiótico la amoxilina  días cada h y como nuevo vete a tomar por el lado oscuro </t>
+          <t xml:space="preserve"> duros</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
-        <is>
-          <t>es</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>1.915496589491147e+18</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>@Farmaenfurecida Amoxilina 500 
-1 cápsula cada 8 horas 2 días 
-Ibuprofeno 600
-1 cápsula cada 8 horas 4 días 
-Y ya...</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>April 24, 2025 at 08:02 PM</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> amoxilina   cápsula cada  horas  días ibuprofeno   cápsula cada  horas  días y ya </t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>es</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>1.91548958975971e+18</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>@madiecedes gracas a Deus</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>April 24, 2025 at 07:34 PM</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> gracas a deus</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>es</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>1.915423938986885e+18</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>@madiecedes so qm copia</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>April 24, 2025 at 03:13 PM</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> so qm copia</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
         <is>
           <t>es</t>
         </is>

</xml_diff>